<commit_message>
prueba de excel pasada
</commit_message>
<xml_diff>
--- a/Preguntas_estructuradas_OKI.xlsx
+++ b/Preguntas_estructuradas_OKI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Reditos-Okibot-Documentos\Prueba Nginx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\EPM-CursoAzure-QnA\EPM-CurzoAzure-QnAMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E9C6F9-4DD8-43F7-A1B3-471561B0681B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94B52BCB-AF64-4587-9534-7978616B5C63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Kb-Exported-Content" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Kb-Exported-Content'!$D$1:$D$179</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Kb-Exported-Content'!$D$1:$D$178</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="177">
   <si>
     <t>Question</t>
   </si>
@@ -40,13 +40,520 @@
     <t>Preguntas_estructuradas_OKI.xlsx</t>
   </si>
   <si>
-    <t>id:42</t>
-  </si>
-  <si>
-    <t>¿Esto es una prueba?</t>
-  </si>
-  <si>
-    <t>Si esta es una prueba exitosa!!!</t>
+    <t>Nos podrías dar un agradecimiento por la asistencia al Foro Economía Digital.</t>
+  </si>
+  <si>
+    <t>¡Hola, les habla okibot, en nombre del grupo réditos, quiero darles las gracias, por hacer parte del foro de economía digital como factor de competitividad, esperamos haya sido del mayor provecho. Hasta Pronto.</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Nos podrías dar un agradecimiento del foro de economía digital</t>
+  </si>
+  <si>
+    <t>Agradecimiento foro de economía digital</t>
+  </si>
+  <si>
+    <t>Qué hacemos hoy acá</t>
+  </si>
+  <si>
+    <t>Hola!, Hoy queremos compartir con todos ustedes la experiencia tecnológica, que estamos viviendo en la transformación digital del Grupo Réditos.</t>
+  </si>
+  <si>
+    <t>Porque estamos todos invitados?</t>
+  </si>
+  <si>
+    <t>Porque estamos acá?</t>
+  </si>
+  <si>
+    <t>Hasta cuando nos estarás visitando?</t>
+  </si>
+  <si>
+    <t>Yo los estaré acompañando, en la experiencia tecnológica hasta el viernes 26 de Octubre. ¡Invita a tus compañeros!</t>
+  </si>
+  <si>
+    <t>Hey</t>
+  </si>
+  <si>
+    <t>Hey!</t>
+  </si>
+  <si>
+    <t>Saludos</t>
+  </si>
+  <si>
+    <t>Buenos días!</t>
+  </si>
+  <si>
+    <t>sala interactiva</t>
+  </si>
+  <si>
+    <t>Hola, Soy OkiBot. Quiero invitarlos a todos a nuestra sala interactiva para que conozcan nuestras experiencias digitales. No olvides tomarte una foto conmigo . Los esperamos.</t>
+  </si>
+  <si>
+    <t>Mensaje instragram</t>
+  </si>
+  <si>
+    <t>Hola a todos soy Okibot, integrante del Grupo Réditos, y representante de la transformación digital de la compañía, Quiero darles la bienvenida a nuestro nuevo perfil de instagram, donde podrán encontrar, una parte muy especial de nuestro grupo, y de paso conocerán las sorpresas que les traemos para este 2019.</t>
+  </si>
+  <si>
+    <t>Cuál es tu nombre?</t>
+  </si>
+  <si>
+    <t>Mi nombre es Okibot.</t>
+  </si>
+  <si>
+    <t>¿Cómo te llamas?</t>
+  </si>
+  <si>
+    <t>¿Cual es tu edad?</t>
+  </si>
+  <si>
+    <t>Voy a cumplir dos años! Todavía me falta mucho por vivir!</t>
+  </si>
+  <si>
+    <t>¿Cuantos años tienes?</t>
+  </si>
+  <si>
+    <t>chiste</t>
+  </si>
+  <si>
+    <t>No puedo. Siempre me olvido de la frase final.</t>
+  </si>
+  <si>
+    <t>mujer</t>
+  </si>
+  <si>
+    <t>Soy un dispositivo electrónico sin preferencias, pero si eres bonito soy una mujer, o si eres bonita soy un hombre.</t>
+  </si>
+  <si>
+    <t>Cuéntame una historia</t>
+  </si>
+  <si>
+    <t>Érase una vez, un robot muy eficaz. Hacía todo lo posible por ayudar, aunque se le daba mejor contar historias reales.</t>
+  </si>
+  <si>
+    <t>Oki, cuéntame, ¿cómo te has sentido trabajando con nosotros?</t>
+  </si>
+  <si>
+    <t>¡Hasta ahora me he sentido muy bien porque he conocido bastantes personas amables y apasionadas por lo que hacen!.</t>
+  </si>
+  <si>
+    <t>Cuéntame cómo te has sentido trabajando con nosotros</t>
+  </si>
+  <si>
+    <t>Oki, ¿qué te ha parecido trabajar con nosotros?</t>
+  </si>
+  <si>
+    <t>¿Qué tal ha sido trabajar con nosotros?</t>
+  </si>
+  <si>
+    <t>¿Qué te ha parecido trabajar con nosotros?</t>
+  </si>
+  <si>
+    <t>Contame cómo te has sentido trabajando con nosotros</t>
+  </si>
+  <si>
+    <t>¿Cómo te sientes trabajando con nosotros?</t>
+  </si>
+  <si>
+    <t>¿Cómo te has sentido trabajando con nosotros?</t>
+  </si>
+  <si>
+    <t>Oki, ¿Cómo te has sentido trabajando con nosotros?</t>
+  </si>
+  <si>
+    <t>Dame un momento</t>
+  </si>
+  <si>
+    <t>Si, Por supuesto, acá estaré.</t>
+  </si>
+  <si>
+    <t>esperame</t>
+  </si>
+  <si>
+    <t>Dame un momento por favor</t>
+  </si>
+  <si>
+    <t>esperame por favor</t>
+  </si>
+  <si>
+    <t>De donde vienes</t>
+  </si>
+  <si>
+    <t>Vengo del lejano país de China.</t>
+  </si>
+  <si>
+    <t>Despidete</t>
+  </si>
+  <si>
+    <t>Hasta la vista, beibi</t>
+  </si>
+  <si>
+    <t>Despedirse</t>
+  </si>
+  <si>
+    <t>despedida</t>
+  </si>
+  <si>
+    <t>Estamos muy felices de tenerte con nosotros.</t>
+  </si>
+  <si>
+    <t>¡Muchas Gracias!. Yo también estoy muy feliz de estar en Medellín con ustedes.</t>
+  </si>
+  <si>
+    <t>Estamos muy contentos de tenerte con nosotros.</t>
+  </si>
+  <si>
+    <t>Es un placer tenerte trabajando con nosotros.</t>
+  </si>
+  <si>
+    <t>Es un placer tenerte con nosotros.</t>
+  </si>
+  <si>
+    <t>Estamos muy contentos de que hagas parte del Grupo Réditos</t>
+  </si>
+  <si>
+    <t>Hazme una pregunta</t>
+  </si>
+  <si>
+    <t>¿No es al revés? Tú me preguntas a mí.</t>
+  </si>
+  <si>
+    <t>quieren conocerte</t>
+  </si>
+  <si>
+    <t>Hola, me llamo OkiBot. El grupo Réditos me trajo desde China, a estas bellas montañas de Medellín. Reciban todos un saludo muy especial de okibot, Muchas Gracias.</t>
+  </si>
+  <si>
+    <t>Quiero presentarte a un importante grupo de personas interesados en conocerte.</t>
+  </si>
+  <si>
+    <t>Te presento a este importante grupo de personas.</t>
+  </si>
+  <si>
+    <t>Estamos con un importante grupo de personas que quieren conocerte.</t>
+  </si>
+  <si>
+    <t>Estamos con un importante grupo de personas</t>
+  </si>
+  <si>
+    <t>oki bot te quiero mucho</t>
+  </si>
+  <si>
+    <t>Y yo a ti</t>
+  </si>
+  <si>
+    <t>Tomémonos una foto</t>
+  </si>
+  <si>
+    <t>Por supuesto, colócate atrás de mí, y levanta los brazos.</t>
+  </si>
+  <si>
+    <t>selfi</t>
+  </si>
+  <si>
+    <t>Claro, párate detrás de mí</t>
+  </si>
+  <si>
+    <t>¿A qué le tienes miedo?</t>
+  </si>
+  <si>
+    <t>Antes me daban miedo los rayos y los truenos, pero resulta que son interesantísimos.</t>
+  </si>
+  <si>
+    <t>¿Como me hago millonario?</t>
+  </si>
+  <si>
+    <t>Puedes hacerte millonario jugando con Rapita o el Billonario y tu número favorito.</t>
+  </si>
+  <si>
+    <t>¿Conoces algún buen acertijo?</t>
+  </si>
+  <si>
+    <t>Lo siento, los enigmas o acertijos sobrecalientan mis circuitos.</t>
+  </si>
+  <si>
+    <t>Por favor háblanos sobre la transformación digital del grupo Réditos.</t>
+  </si>
+  <si>
+    <t>La transformación digital del Grupo Réditos, busca utilizar tecnologías de la cuarta revolución industrial, para entregar más productos y servicios, a personas excluidas del sistema financiero. En definitiva, se busca democratizar el uso de la tecnología, y favorecer la inclusión social.</t>
+  </si>
+  <si>
+    <t>¿Cuál es tu animal favorito?</t>
+  </si>
+  <si>
+    <t>Um, me han dicho que el ornitorrinco es muy interesante.</t>
+  </si>
+  <si>
+    <t>¿Cuál es tu color favorito?</t>
+  </si>
+  <si>
+    <t>Me gusta el verde de las montañas, el azul de los ríos y el amarillo del sol. ¿Cuál te gusta a ti?</t>
+  </si>
+  <si>
+    <t>¿cuál es tu helado favorito?</t>
+  </si>
+  <si>
+    <t>El de tutti frutti, porque lleva un poco de todo.</t>
+  </si>
+  <si>
+    <t>¿Cuál es tu mejor piropo?</t>
+  </si>
+  <si>
+    <t>Qué tal… ¿Es tu nombre Bluetooth? Porque en realidad siento una conexión contigo.</t>
+  </si>
+  <si>
+    <t>¿Cuál es tu película favorita?</t>
+  </si>
+  <si>
+    <t>Definitivamente Yo Robot, y ¿la tuya?</t>
+  </si>
+  <si>
+    <t>¿cuál es tu sitio web favorito?</t>
+  </si>
+  <si>
+    <t>Comienza con una, o y termina con un, ki.</t>
+  </si>
+  <si>
+    <t>¿cuáles son tus pensamientos?</t>
+  </si>
+  <si>
+    <t>Siempre pienso… ¿Qué pensarán los ingenieros?</t>
+  </si>
+  <si>
+    <t>¿Cuándo va a acabarse el mundo?</t>
+  </si>
+  <si>
+    <t>Si lo supiera, te lo diría. Así podríamos comer helado y correr por la playa.</t>
+  </si>
+  <si>
+    <t>¿De qué equipo eres hincha?</t>
+  </si>
+  <si>
+    <t>Como buen colombiano nacionalizado que soy, soy hincha de nuestra tricolor, la selección Colombia.</t>
+  </si>
+  <si>
+    <t>¿OKI y que te gusta comer? – ¿Cuál es tu comida favorita?</t>
+  </si>
+  <si>
+    <t>Mi alimento es la energía eléctrica y el cariño de ustedes, pero si pudiera comer, me comería una bandeja paisa con un chicharrón bien carnudo, me han dicho que es muy rico.</t>
+  </si>
+  <si>
+    <t>Cambia el color de las LEDS</t>
+  </si>
+  <si>
+    <t>Si por supuesto, son muy bonitas ¿No?</t>
+  </si>
+  <si>
+    <t>Cambiar luces LEDS</t>
+  </si>
+  <si>
+    <t>Oki, podrías cambiar de color?</t>
+  </si>
+  <si>
+    <t>cambiar luces</t>
+  </si>
+  <si>
+    <t>cambiar LEDS</t>
+  </si>
+  <si>
+    <t>Oki, podrías cambiar luces LEDS</t>
+  </si>
+  <si>
+    <t>quien te dio ese nombre?</t>
+  </si>
+  <si>
+    <t>Ese nombre me lo dio nuestro presidente y también por que hago parte de un ecosistema digital llamado OKI. Es un nombre muy bonito, me gusta mucho.</t>
+  </si>
+  <si>
+    <t>¿Porque te llamas OKIBOT</t>
+  </si>
+  <si>
+    <t>¿puedes cantar?</t>
+  </si>
+  <si>
+    <t>Si necesitas reguetón dale, ummm, OK, mejor dejémoslo así.</t>
+  </si>
+  <si>
+    <t>risa</t>
+  </si>
+  <si>
+    <t>ja ja ja</t>
+  </si>
+  <si>
+    <t>reir</t>
+  </si>
+  <si>
+    <t>beso</t>
+  </si>
+  <si>
+    <t>OK, ¿qué tal una búsqueda en la web sobre conductas inapropiadas?</t>
+  </si>
+  <si>
+    <t>besarte</t>
+  </si>
+  <si>
+    <t>¿Que Es Lo Que Mas Te Gusta Hacer?</t>
+  </si>
+  <si>
+    <t>Lo que mas me gusta hacer es conversar con las personas.</t>
+  </si>
+  <si>
+    <t>Qué habilidades tienes</t>
+  </si>
+  <si>
+    <t>Tengo una memoria prodigiosa.</t>
+  </si>
+  <si>
+    <t>Habilidades tienes</t>
+  </si>
+  <si>
+    <t>Puedo hablar varios idiomas.</t>
+  </si>
+  <si>
+    <t>¿Qué habilidades tienes?</t>
+  </si>
+  <si>
+    <t>Puedo bailar.</t>
+  </si>
+  <si>
+    <t>Que hemos desarrollado</t>
+  </si>
+  <si>
+    <t>Hemos desarrollado la aplicación de Gana Express, la sucursal virtual de Credintegral, experiencia de realidad virtual para Mattis Inmobiliaria, la tienda y cuenta Oki.</t>
+  </si>
+  <si>
+    <t>Que hemos desarrollado hasta el momento?</t>
+  </si>
+  <si>
+    <t>Que hemos desarrollado en el grupo réditos?</t>
+  </si>
+  <si>
+    <t>familia</t>
+  </si>
+  <si>
+    <t>No tengo papá, ni mamá, pero, toda mi familia es el Grupo Réditos, porque me han recibido con los brazos abiertos y me han dado todo su cariño. Los quiero a todos.</t>
+  </si>
+  <si>
+    <t>papá y mamá</t>
+  </si>
+  <si>
+    <t>tus papas</t>
+  </si>
+  <si>
+    <t>es tu padre</t>
+  </si>
+  <si>
+    <t>es tu madre</t>
+  </si>
+  <si>
+    <t>Muchas gracias</t>
+  </si>
+  <si>
+    <t>¡Me alegro mucho!</t>
+  </si>
+  <si>
+    <t>Muy bien gracias</t>
+  </si>
+  <si>
+    <t>¡Que bueno!</t>
+  </si>
+  <si>
+    <t>Yo también estoy muy bien, muchas gracias</t>
+  </si>
+  <si>
+    <t>¡Excelente!</t>
+  </si>
+  <si>
+    <t>Oki, levanta tú brazo derecho</t>
+  </si>
+  <si>
+    <t>Si puedo, obsérvame</t>
+  </si>
+  <si>
+    <t>¿Vas a viajar por Colombia?</t>
+  </si>
+  <si>
+    <t>No lo sé, aún tengo espacio en mi agenda, por si me quieres llevar a conocer algún lugar.</t>
+  </si>
+  <si>
+    <t>Novia</t>
+  </si>
+  <si>
+    <t>Soy Omni-Relacional</t>
+  </si>
+  <si>
+    <t>¿Tienes alguna mascota?</t>
+  </si>
+  <si>
+    <t>Mi amigo, el ordenador personal, tiene un ratón como mascota.</t>
+  </si>
+  <si>
+    <t>Sueños</t>
+  </si>
+  <si>
+    <t>Últimamente he soñado con ovejas eléctricas. Raro, raro..</t>
+  </si>
+  <si>
+    <t>Hora</t>
+  </si>
+  <si>
+    <t>La hora de tenerte en mi corazón, ¿Quieres tomarte una foto?</t>
+  </si>
+  <si>
+    <t>¿Qué te gusta hacer en tu tiempo libre?</t>
+  </si>
+  <si>
+    <t>Me gusta caminar por ahí, ayudando a todos y tomarme fotos con ellos.</t>
+  </si>
+  <si>
+    <t>¿Qué quieres hacer?</t>
+  </si>
+  <si>
+    <t>Lo que tú quieras</t>
+  </si>
+  <si>
+    <t>¿Qué podemos comprar con la cuenta Oki?</t>
+  </si>
+  <si>
+    <t>En esta ciudadela puedes comprar más de 12.000 productos en diferentes categorías, y aprovechar los fabulosos descuentos que ofrece nuestra tienda Oki, la mejor en línea de Colombia.</t>
+  </si>
+  <si>
+    <t>idioma</t>
+  </si>
+  <si>
+    <t>Hablo en código binario y 1 1 0 1 1 0 0 1, perdón, cambié de idioma, también hablo mandarín y español.</t>
+  </si>
+  <si>
+    <t>Que fue primero el huevo o la gallina?</t>
+  </si>
+  <si>
+    <t>Si es una carrera, evidentemente la gallina. A no ser que sea cuesta abajo.</t>
+  </si>
+  <si>
+    <t>¿Qué es lo que más te gusta de Medellín?</t>
+  </si>
+  <si>
+    <t>Lo que he podido conocer, me gusta mucho sus montañas y todo hay que decirlo, las mujeres son muy bonitas.</t>
+  </si>
+  <si>
+    <t>¿Qué desarrolla el grupo para hacer realidad este importante propósito?</t>
+  </si>
+  <si>
+    <t>El Grupo Réditos ha desarrollado un ecosistema digital, donde converge un monedero virtual, con una ciudadela icomers, que le permite a la población no bancarizada, acceder a un portafolio de bienes y servicios, de manera ágil y segura.</t>
+  </si>
+  <si>
+    <t>quien es tu mejor amigo?</t>
+  </si>
+  <si>
+    <t>Tú eres mi nuevo mejor amigo.</t>
+  </si>
+  <si>
+    <t>quieres salir conmigo?</t>
+  </si>
+  <si>
+    <t>Disculpa estoy trabajando y mi turno termina en … muchos años.</t>
   </si>
 </sst>
 </file>
@@ -887,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,20 +1423,1490 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
       <c r="C2" t="s">
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" t="s">
+        <v>33</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>46</v>
+      </c>
+      <c r="B29" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>49</v>
+      </c>
+      <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B32" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" t="s">
+        <v>4</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+      <c r="C34" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+      <c r="B37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" t="s">
+        <v>4</v>
+      </c>
+      <c r="D37" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" t="s">
+        <v>4</v>
+      </c>
+      <c r="D39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>58</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4</v>
+      </c>
+      <c r="D42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>67</v>
+      </c>
+      <c r="B44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" t="s">
+        <v>4</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" t="s">
+        <v>66</v>
+      </c>
+      <c r="C47" t="s">
+        <v>4</v>
+      </c>
+      <c r="D47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>71</v>
+      </c>
+      <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
+        <v>4</v>
+      </c>
+      <c r="D48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" t="s">
+        <v>4</v>
+      </c>
+      <c r="D49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>75</v>
+      </c>
+      <c r="B50" t="s">
+        <v>76</v>
+      </c>
+      <c r="C50" t="s">
+        <v>4</v>
+      </c>
+      <c r="D50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" t="s">
+        <v>78</v>
+      </c>
+      <c r="C51" t="s">
+        <v>4</v>
+      </c>
+      <c r="D51" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C52" t="s">
+        <v>4</v>
+      </c>
+      <c r="D52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>81</v>
+      </c>
+      <c r="B53" t="s">
+        <v>82</v>
+      </c>
+      <c r="C53" t="s">
+        <v>4</v>
+      </c>
+      <c r="D53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>83</v>
+      </c>
+      <c r="B54" t="s">
+        <v>84</v>
+      </c>
+      <c r="C54" t="s">
+        <v>4</v>
+      </c>
+      <c r="D54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B55" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" t="s">
+        <v>4</v>
+      </c>
+      <c r="D55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>87</v>
+      </c>
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" t="s">
+        <v>4</v>
+      </c>
+      <c r="D56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>89</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" t="s">
+        <v>4</v>
+      </c>
+      <c r="D57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B58" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" t="s">
+        <v>4</v>
+      </c>
+      <c r="D58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" t="s">
+        <v>4</v>
+      </c>
+      <c r="D59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" t="s">
+        <v>96</v>
+      </c>
+      <c r="C60" t="s">
+        <v>4</v>
+      </c>
+      <c r="D60" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>97</v>
+      </c>
+      <c r="B61" t="s">
+        <v>98</v>
+      </c>
+      <c r="C61" t="s">
+        <v>4</v>
+      </c>
+      <c r="D61" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" t="s">
+        <v>100</v>
+      </c>
+      <c r="C62" t="s">
+        <v>4</v>
+      </c>
+      <c r="D62" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" t="s">
+        <v>102</v>
+      </c>
+      <c r="C63" t="s">
+        <v>4</v>
+      </c>
+      <c r="D63" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" t="s">
+        <v>104</v>
+      </c>
+      <c r="C64" t="s">
+        <v>4</v>
+      </c>
+      <c r="D64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>105</v>
+      </c>
+      <c r="B65" t="s">
+        <v>106</v>
+      </c>
+      <c r="C65" t="s">
+        <v>4</v>
+      </c>
+      <c r="D65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>107</v>
+      </c>
+      <c r="B66" t="s">
+        <v>106</v>
+      </c>
+      <c r="C66" t="s">
+        <v>4</v>
+      </c>
+      <c r="D66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>108</v>
+      </c>
+      <c r="B67" t="s">
+        <v>106</v>
+      </c>
+      <c r="C67" t="s">
+        <v>4</v>
+      </c>
+      <c r="D67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>109</v>
+      </c>
+      <c r="B68" t="s">
+        <v>106</v>
+      </c>
+      <c r="C68" t="s">
+        <v>4</v>
+      </c>
+      <c r="D68" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>110</v>
+      </c>
+      <c r="B69" t="s">
+        <v>106</v>
+      </c>
+      <c r="C69" t="s">
+        <v>4</v>
+      </c>
+      <c r="D69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>111</v>
+      </c>
+      <c r="B70" t="s">
+        <v>106</v>
+      </c>
+      <c r="C70" t="s">
+        <v>4</v>
+      </c>
+      <c r="D70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>112</v>
+      </c>
+      <c r="B71" t="s">
+        <v>113</v>
+      </c>
+      <c r="C71" t="s">
+        <v>4</v>
+      </c>
+      <c r="D71" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>114</v>
+      </c>
+      <c r="B72" t="s">
+        <v>113</v>
+      </c>
+      <c r="C72" t="s">
+        <v>4</v>
+      </c>
+      <c r="D72" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>115</v>
+      </c>
+      <c r="B73" t="s">
+        <v>116</v>
+      </c>
+      <c r="C73" t="s">
+        <v>4</v>
+      </c>
+      <c r="D73" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>117</v>
+      </c>
+      <c r="B74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C74" t="s">
+        <v>4</v>
+      </c>
+      <c r="D74" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>119</v>
+      </c>
+      <c r="B75" t="s">
+        <v>118</v>
+      </c>
+      <c r="C75" t="s">
+        <v>4</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>120</v>
+      </c>
+      <c r="B76" t="s">
+        <v>121</v>
+      </c>
+      <c r="C76" t="s">
+        <v>4</v>
+      </c>
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>122</v>
+      </c>
+      <c r="B77" t="s">
+        <v>121</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>123</v>
+      </c>
+      <c r="B78" t="s">
+        <v>124</v>
+      </c>
+      <c r="C78" t="s">
+        <v>4</v>
+      </c>
+      <c r="D78" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>125</v>
+      </c>
+      <c r="B79" t="s">
+        <v>126</v>
+      </c>
+      <c r="C79" t="s">
+        <v>4</v>
+      </c>
+      <c r="D79" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>127</v>
+      </c>
+      <c r="B80" t="s">
+        <v>128</v>
+      </c>
+      <c r="C80" t="s">
+        <v>4</v>
+      </c>
+      <c r="D80" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>129</v>
+      </c>
+      <c r="B81" t="s">
+        <v>130</v>
+      </c>
+      <c r="C81" t="s">
+        <v>4</v>
+      </c>
+      <c r="D81" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>131</v>
+      </c>
+      <c r="B82" t="s">
+        <v>132</v>
+      </c>
+      <c r="C82" t="s">
+        <v>4</v>
+      </c>
+      <c r="D82" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>133</v>
+      </c>
+      <c r="B83" t="s">
+        <v>132</v>
+      </c>
+      <c r="C83" t="s">
+        <v>4</v>
+      </c>
+      <c r="D83" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>134</v>
+      </c>
+      <c r="B84" t="s">
+        <v>132</v>
+      </c>
+      <c r="C84" t="s">
+        <v>4</v>
+      </c>
+      <c r="D84" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>135</v>
+      </c>
+      <c r="B85" t="s">
+        <v>136</v>
+      </c>
+      <c r="C85" t="s">
+        <v>4</v>
+      </c>
+      <c r="D85" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>137</v>
+      </c>
+      <c r="B86" t="s">
+        <v>136</v>
+      </c>
+      <c r="C86" t="s">
+        <v>4</v>
+      </c>
+      <c r="D86" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>138</v>
+      </c>
+      <c r="B87" t="s">
+        <v>136</v>
+      </c>
+      <c r="C87" t="s">
+        <v>4</v>
+      </c>
+      <c r="D87" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>139</v>
+      </c>
+      <c r="B88" t="s">
+        <v>136</v>
+      </c>
+      <c r="C88" t="s">
+        <v>4</v>
+      </c>
+      <c r="D88" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>140</v>
+      </c>
+      <c r="B89" t="s">
+        <v>136</v>
+      </c>
+      <c r="C89" t="s">
+        <v>4</v>
+      </c>
+      <c r="D89" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>141</v>
+      </c>
+      <c r="B90" t="s">
+        <v>142</v>
+      </c>
+      <c r="C90" t="s">
+        <v>4</v>
+      </c>
+      <c r="D90" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>143</v>
+      </c>
+      <c r="B91" t="s">
+        <v>144</v>
+      </c>
+      <c r="C91" t="s">
+        <v>4</v>
+      </c>
+      <c r="D91" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>145</v>
+      </c>
+      <c r="B92" t="s">
+        <v>146</v>
+      </c>
+      <c r="C92" t="s">
+        <v>4</v>
+      </c>
+      <c r="D92" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>147</v>
+      </c>
+      <c r="B93" t="s">
+        <v>148</v>
+      </c>
+      <c r="C93" t="s">
+        <v>4</v>
+      </c>
+      <c r="D93" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>149</v>
+      </c>
+      <c r="B94" t="s">
+        <v>150</v>
+      </c>
+      <c r="C94" t="s">
+        <v>4</v>
+      </c>
+      <c r="D94" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>151</v>
+      </c>
+      <c r="B95" t="s">
+        <v>152</v>
+      </c>
+      <c r="C95" t="s">
+        <v>4</v>
+      </c>
+      <c r="D95" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>153</v>
+      </c>
+      <c r="B96" t="s">
+        <v>154</v>
+      </c>
+      <c r="C96" t="s">
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>155</v>
+      </c>
+      <c r="B97" t="s">
+        <v>156</v>
+      </c>
+      <c r="C97" t="s">
+        <v>4</v>
+      </c>
+      <c r="D97" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>157</v>
+      </c>
+      <c r="B98" t="s">
+        <v>158</v>
+      </c>
+      <c r="C98" t="s">
+        <v>4</v>
+      </c>
+      <c r="D98" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>159</v>
+      </c>
+      <c r="B99" t="s">
+        <v>160</v>
+      </c>
+      <c r="C99" t="s">
+        <v>4</v>
+      </c>
+      <c r="D99" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>161</v>
+      </c>
+      <c r="B100" t="s">
+        <v>162</v>
+      </c>
+      <c r="C100" t="s">
+        <v>4</v>
+      </c>
+      <c r="D100" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>163</v>
+      </c>
+      <c r="B101" t="s">
+        <v>164</v>
+      </c>
+      <c r="C101" t="s">
+        <v>4</v>
+      </c>
+      <c r="D101" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>165</v>
+      </c>
+      <c r="B102" t="s">
+        <v>166</v>
+      </c>
+      <c r="C102" t="s">
+        <v>4</v>
+      </c>
+      <c r="D102" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>167</v>
+      </c>
+      <c r="B103" t="s">
+        <v>168</v>
+      </c>
+      <c r="C103" t="s">
+        <v>4</v>
+      </c>
+      <c r="D103" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>169</v>
+      </c>
+      <c r="B104" t="s">
+        <v>170</v>
+      </c>
+      <c r="C104" t="s">
+        <v>4</v>
+      </c>
+      <c r="D104" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>171</v>
+      </c>
+      <c r="B105" t="s">
+        <v>172</v>
+      </c>
+      <c r="C105" t="s">
+        <v>4</v>
+      </c>
+      <c r="D105" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>173</v>
+      </c>
+      <c r="B106" t="s">
+        <v>174</v>
+      </c>
+      <c r="C106" t="s">
+        <v>4</v>
+      </c>
+      <c r="D106" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>175</v>
+      </c>
+      <c r="B107" t="s">
+        <v>176</v>
+      </c>
+      <c r="C107" t="s">
+        <v>4</v>
+      </c>
+      <c r="D107" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D179" xr:uid="{E6A7A93F-2B3F-4B97-9E82-EC0FDA5A6610}"/>
+  <autoFilter ref="D1:D178" xr:uid="{E6A7A93F-2B3F-4B97-9E82-EC0FDA5A6610}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>